<commit_message>
first two sliders working!
</commit_message>
<xml_diff>
--- a/ghg-app/Project_Figures.xlsx
+++ b/ghg-app/Project_Figures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45084d7f136e201d/Documents/372-project/ghg-app/ghg-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{49CF4CDE-090B-43BF-8E3C-85C4D8F67711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBB5E7F8-C4EA-4E81-8D3D-ED01DE3F56A0}"/>
+  <xr:revisionPtr revIDLastSave="373" documentId="8_{49CF4CDE-090B-43BF-8E3C-85C4D8F67711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72C94FB6-CBC8-4550-9EDE-FA3591ED3B7A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{97376A2B-792E-4B38-A661-81DC03B910A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{97376A2B-792E-4B38-A661-81DC03B910A2}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Students %" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="34">
   <si>
     <t>Emissions</t>
   </si>
@@ -80,6 +80,69 @@
   <si>
     <t>offsets/insets</t>
   </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>other Adjusted</t>
+  </si>
+  <si>
+    <t>Student commuting</t>
+  </si>
+  <si>
+    <t>Business Travel - accomodation</t>
+  </si>
+  <si>
+    <t>Steam &amp; MTHW - biomass (incl losses)</t>
+  </si>
+  <si>
+    <t>Business Travel - mileage, taxis and shuttles</t>
+  </si>
+  <si>
+    <t>Fugitive Emissions - refrigerants</t>
+  </si>
+  <si>
+    <t>Mobile Combustion - diesel, petrol, pcard &amp; marine</t>
+  </si>
+  <si>
+    <t>Stationary Combustion - biomass</t>
+  </si>
+  <si>
+    <t>Purchased Goods and Services - water</t>
+  </si>
+  <si>
+    <t>Stationary Combustion - diesel</t>
+  </si>
+  <si>
+    <t>Employee Commuting -public transport</t>
+  </si>
+  <si>
+    <t>Construction &amp; demolition</t>
+  </si>
+  <si>
+    <t>other adjusted</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Scenario_5</t>
+  </si>
+  <si>
+    <t>Scenario_4</t>
+  </si>
+  <si>
+    <t>Scenario_3</t>
+  </si>
+  <si>
+    <t>Scenario_2</t>
+  </si>
+  <si>
+    <t>Scenario_1</t>
+  </si>
 </sst>
 </file>
 
@@ -109,12 +172,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -140,6 +209,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,10 +927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC311DF2-2015-4D96-96D3-502F22096FE8}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,6 +1271,758 @@
         <v>1067.6144898840566</v>
       </c>
     </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2025</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2026</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2027</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2028</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2029</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2030</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2031</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-0.05</v>
+      </c>
+      <c r="D10">
+        <v>-0.2</v>
+      </c>
+      <c r="E10">
+        <v>-0.25</v>
+      </c>
+      <c r="F10">
+        <v>-0.3</v>
+      </c>
+      <c r="G10">
+        <v>-0.35</v>
+      </c>
+      <c r="H10">
+        <v>-0.4</v>
+      </c>
+      <c r="I10">
+        <v>-0.45</v>
+      </c>
+      <c r="J10">
+        <v>-0.5</v>
+      </c>
+      <c r="K10">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="L10">
+        <v>-0.6</v>
+      </c>
+      <c r="M10">
+        <v>-0.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-0.05</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="H11" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="I11" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="J11" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K11" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="L11" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="M11" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-0.05</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="F12" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="G12" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="H12" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="I12" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="J12" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K12" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="L12" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="M12" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>-0.05</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="F13" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="G13" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="H13" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="I13" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="J13" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K13" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="L13" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="M13" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>-0.1</v>
+      </c>
+      <c r="D14">
+        <v>-0.15</v>
+      </c>
+      <c r="E14">
+        <v>-0.2</v>
+      </c>
+      <c r="F14">
+        <v>-0.25</v>
+      </c>
+      <c r="G14">
+        <v>-0.3</v>
+      </c>
+      <c r="H14">
+        <v>-0.35</v>
+      </c>
+      <c r="I14">
+        <v>-0.4</v>
+      </c>
+      <c r="J14">
+        <v>-0.45</v>
+      </c>
+      <c r="K14">
+        <v>-0.5</v>
+      </c>
+      <c r="L14">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="M14">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>-6.3681466653225147E-2</v>
+      </c>
+      <c r="D15">
+        <v>-7.8121111079378358E-2</v>
+      </c>
+      <c r="E15">
+        <v>-9.4065602348630262E-2</v>
+      </c>
+      <c r="F15">
+        <v>-0.10875550657245797</v>
+      </c>
+      <c r="G15">
+        <v>-0.10477499797785675</v>
+      </c>
+      <c r="H15">
+        <v>-0.11546772696052705</v>
+      </c>
+      <c r="I15">
+        <v>-0.12585471368474122</v>
+      </c>
+      <c r="J15">
+        <v>-0.13594260692112645</v>
+      </c>
+      <c r="K15">
+        <v>-0.14573904403040494</v>
+      </c>
+      <c r="L15">
+        <v>-0.15377292673079804</v>
+      </c>
+      <c r="M15">
+        <v>-0.16145478228094809</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2025</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2026</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2027</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2028</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2029</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2030</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2031</v>
+      </c>
+      <c r="M16" s="1">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-0.05</v>
+      </c>
+      <c r="D17" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="G17" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="H17" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="I17" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="J17" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="K17" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="L17" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="M17" s="5">
+        <v>-0.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>-0.05</v>
+      </c>
+      <c r="D20" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="G20" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="H20" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="I20" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="J20" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K20" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="L20" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="M20" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>-0.05</v>
+      </c>
+      <c r="D21" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="E21" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="F21" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="G21" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="H21" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="I21" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="J21" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K21" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="L21" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="M21" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>-0.05</v>
+      </c>
+      <c r="D22" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="F22" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="G22" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="H22" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="I22" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="J22" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K22" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="L22" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="M22" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="D24" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="E24" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="F24" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="G24" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="H24" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="I24" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="J24" s="5">
+        <v>-0.45</v>
+      </c>
+      <c r="K24" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="L24" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="M24" s="5">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0</v>
+      </c>
+      <c r="M25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0.52495066036182003</v>
+      </c>
+      <c r="D26">
+        <v>0.5297996513825517</v>
+      </c>
+      <c r="E26">
+        <v>0.52959560495957025</v>
+      </c>
+      <c r="F26">
+        <v>0.52952381356074885</v>
+      </c>
+      <c r="G26">
+        <v>0.52865644367315678</v>
+      </c>
+      <c r="H26">
+        <v>0.52835516080470313</v>
+      </c>
+      <c r="I26">
+        <v>0.52805618918539432</v>
+      </c>
+      <c r="J26">
+        <v>0.52776006719664403</v>
+      </c>
+      <c r="K26">
+        <v>0.5274673122257223</v>
+      </c>
+      <c r="L26">
+        <v>0.52706643407296205</v>
+      </c>
+      <c r="M26">
+        <v>0.5266783045958241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1206,15 +2030,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80781A22-78B0-402B-B62D-62368369D652}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="69" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1403,8 +2227,2179 @@
         <v>1067.6144898840566</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2025</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2026</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2027</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2028</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2029</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2030</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2031</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="E11">
+        <v>-9.9999999999999534E-2</v>
+      </c>
+      <c r="F11">
+        <v>-0.14999999999999958</v>
+      </c>
+      <c r="G11">
+        <v>-0.19999999999999962</v>
+      </c>
+      <c r="H11">
+        <v>-0.24999999999999967</v>
+      </c>
+      <c r="I11">
+        <v>-0.49999999999999989</v>
+      </c>
+      <c r="J11">
+        <v>-0.74999999999999956</v>
+      </c>
+      <c r="K11">
+        <v>-1</v>
+      </c>
+      <c r="L11">
+        <v>-1</v>
+      </c>
+      <c r="M11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>-0.02</v>
+      </c>
+      <c r="F15">
+        <v>-0.04</v>
+      </c>
+      <c r="G15">
+        <v>-0.06</v>
+      </c>
+      <c r="H15">
+        <v>-0.08</v>
+      </c>
+      <c r="I15">
+        <v>-0.1</v>
+      </c>
+      <c r="J15">
+        <v>-0.12</v>
+      </c>
+      <c r="K15">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L15">
+        <v>-0.16</v>
+      </c>
+      <c r="M15">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-0.04</v>
+      </c>
+      <c r="G20" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="H20" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I20" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="J20" s="5">
+        <v>-0.12</v>
+      </c>
+      <c r="K20" s="5">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L20" s="5">
+        <v>-0.16</v>
+      </c>
+      <c r="M20" s="5">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="F21" s="5">
+        <v>-0.04</v>
+      </c>
+      <c r="G21" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="H21" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I21" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="J21" s="5">
+        <v>-0.12</v>
+      </c>
+      <c r="K21" s="5">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L21" s="5">
+        <v>-0.16</v>
+      </c>
+      <c r="M21" s="5">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="F23" s="5">
+        <v>-0.04</v>
+      </c>
+      <c r="G23" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="H23" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I23" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="J23" s="5">
+        <v>-0.12</v>
+      </c>
+      <c r="K23" s="5">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L23" s="5">
+        <v>-0.16</v>
+      </c>
+      <c r="M23" s="5">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="5">
+        <v>0</v>
+      </c>
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="F25" s="5">
+        <v>-0.04</v>
+      </c>
+      <c r="G25" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="H25" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I25" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="J25" s="5">
+        <v>-0.12</v>
+      </c>
+      <c r="K25" s="5">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L25" s="5">
+        <v>-0.16</v>
+      </c>
+      <c r="M25" s="5">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5">
+        <v>0</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="F28" s="5">
+        <v>-0.04</v>
+      </c>
+      <c r="G28" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="H28" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I28" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>-0.12</v>
+      </c>
+      <c r="K28" s="5">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L28" s="5">
+        <v>-0.16</v>
+      </c>
+      <c r="M28" s="5">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>-0.02</v>
+      </c>
+      <c r="F29" s="5">
+        <v>-0.04</v>
+      </c>
+      <c r="G29" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="H29" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I29" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="J29" s="5">
+        <v>-0.12</v>
+      </c>
+      <c r="K29" s="5">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="L29" s="5">
+        <v>-0.16</v>
+      </c>
+      <c r="M29" s="5">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>200</v>
+      </c>
+      <c r="C32">
+        <v>200</v>
+      </c>
+      <c r="D32">
+        <v>150</v>
+      </c>
+      <c r="E32">
+        <v>150</v>
+      </c>
+      <c r="F32">
+        <v>150</v>
+      </c>
+      <c r="G32">
+        <v>150</v>
+      </c>
+      <c r="H32">
+        <v>150</v>
+      </c>
+      <c r="I32">
+        <v>150</v>
+      </c>
+      <c r="J32">
+        <v>150</v>
+      </c>
+      <c r="K32">
+        <v>150</v>
+      </c>
+      <c r="L32">
+        <v>151</v>
+      </c>
+      <c r="M32">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>123.74000000000001</v>
+      </c>
+      <c r="D33">
+        <v>116.3156</v>
+      </c>
+      <c r="E33">
+        <v>109.336664</v>
+      </c>
+      <c r="F33">
+        <v>102.77646415999999</v>
+      </c>
+      <c r="G33">
+        <v>96.609876310399983</v>
+      </c>
+      <c r="H33">
+        <v>90.813283731775982</v>
+      </c>
+      <c r="I33">
+        <v>85.364486707869418</v>
+      </c>
+      <c r="J33">
+        <v>80.242617505397249</v>
+      </c>
+      <c r="K33">
+        <v>75.428060455073407</v>
+      </c>
+      <c r="L33">
+        <v>70.902376827769004</v>
+      </c>
+      <c r="M33">
+        <v>66.648234218102857</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>250</v>
+      </c>
+      <c r="C34">
+        <v>287</v>
+      </c>
+      <c r="D34">
+        <v>400</v>
+      </c>
+      <c r="E34">
+        <v>400</v>
+      </c>
+      <c r="F34">
+        <v>400</v>
+      </c>
+      <c r="G34">
+        <v>400</v>
+      </c>
+      <c r="H34">
+        <v>400</v>
+      </c>
+      <c r="I34">
+        <v>400</v>
+      </c>
+      <c r="J34">
+        <v>400</v>
+      </c>
+      <c r="K34">
+        <v>400</v>
+      </c>
+      <c r="L34">
+        <v>400</v>
+      </c>
+      <c r="M34">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>100</v>
+      </c>
+      <c r="C35">
+        <v>150</v>
+      </c>
+      <c r="D35">
+        <v>141</v>
+      </c>
+      <c r="E35">
+        <v>132.54</v>
+      </c>
+      <c r="F35">
+        <v>124.58759999999998</v>
+      </c>
+      <c r="G35">
+        <v>117.11234399999998</v>
+      </c>
+      <c r="H35">
+        <v>110.08560335999998</v>
+      </c>
+      <c r="I35">
+        <v>103.48046715839997</v>
+      </c>
+      <c r="J35">
+        <v>97.27163912889597</v>
+      </c>
+      <c r="K35">
+        <v>91.435340781162211</v>
+      </c>
+      <c r="L35">
+        <v>82.291806703045992</v>
+      </c>
+      <c r="M35">
+        <v>74.062626032741392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>100</v>
+      </c>
+      <c r="C36">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+      <c r="E36">
+        <v>94</v>
+      </c>
+      <c r="F36">
+        <v>88.36</v>
+      </c>
+      <c r="G36">
+        <v>83.058399999999992</v>
+      </c>
+      <c r="H36">
+        <v>78.074895999999981</v>
+      </c>
+      <c r="I36">
+        <v>73.390402239999972</v>
+      </c>
+      <c r="J36">
+        <v>68.986978105599974</v>
+      </c>
+      <c r="K36">
+        <v>64.847759419263966</v>
+      </c>
+      <c r="L36">
+        <v>60.956893854108124</v>
+      </c>
+      <c r="M36">
+        <v>57.299480222861632</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>250</v>
+      </c>
+      <c r="C37">
+        <v>250</v>
+      </c>
+      <c r="D37">
+        <v>235</v>
+      </c>
+      <c r="E37">
+        <v>220.89999999999998</v>
+      </c>
+      <c r="F37">
+        <v>207.64599999999996</v>
+      </c>
+      <c r="G37">
+        <v>195.18723999999995</v>
+      </c>
+      <c r="H37">
+        <v>183.47600559999995</v>
+      </c>
+      <c r="I37">
+        <v>172.46744526399993</v>
+      </c>
+      <c r="J37">
+        <v>162.11939854815992</v>
+      </c>
+      <c r="K37">
+        <v>152.39223463527031</v>
+      </c>
+      <c r="L37">
+        <v>137.15301117174329</v>
+      </c>
+      <c r="M37">
+        <v>123.43771005456897</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>60</v>
+      </c>
+      <c r="C38">
+        <v>66</v>
+      </c>
+      <c r="D38">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>80</v>
+      </c>
+      <c r="F38">
+        <v>100</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>100</v>
+      </c>
+      <c r="I38">
+        <v>100</v>
+      </c>
+      <c r="J38">
+        <v>100</v>
+      </c>
+      <c r="K38">
+        <v>100</v>
+      </c>
+      <c r="L38">
+        <v>100</v>
+      </c>
+      <c r="M38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <v>82</v>
+      </c>
+      <c r="C39">
+        <v>82</v>
+      </c>
+      <c r="D39">
+        <v>77.08</v>
+      </c>
+      <c r="E39">
+        <v>72.455199999999991</v>
+      </c>
+      <c r="F39">
+        <v>68.107887999999988</v>
+      </c>
+      <c r="G39">
+        <v>64.021414719999981</v>
+      </c>
+      <c r="H39">
+        <v>60.180129836799978</v>
+      </c>
+      <c r="I39">
+        <v>56.569322046591978</v>
+      </c>
+      <c r="J39">
+        <v>53.175162723796454</v>
+      </c>
+      <c r="K39">
+        <v>49.984652960368663</v>
+      </c>
+      <c r="L39">
+        <v>46.985573782746542</v>
+      </c>
+      <c r="M39">
+        <v>44.166439355781748</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <v>80</v>
+      </c>
+      <c r="C40">
+        <v>80</v>
+      </c>
+      <c r="D40">
+        <v>75.199999999999989</v>
+      </c>
+      <c r="E40">
+        <v>70.687999999999988</v>
+      </c>
+      <c r="F40">
+        <v>66.446719999999985</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41">
+        <v>50</v>
+      </c>
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="D41">
+        <v>50</v>
+      </c>
+      <c r="E41">
+        <v>50</v>
+      </c>
+      <c r="F41">
+        <v>50</v>
+      </c>
+      <c r="G41">
+        <v>50</v>
+      </c>
+      <c r="H41">
+        <v>50</v>
+      </c>
+      <c r="I41">
+        <v>50</v>
+      </c>
+      <c r="J41">
+        <v>50</v>
+      </c>
+      <c r="K41">
+        <v>50</v>
+      </c>
+      <c r="L41">
+        <v>50</v>
+      </c>
+      <c r="M41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <f>(E32+(E20 *E32))</f>
+        <v>147</v>
+      </c>
+      <c r="F44">
+        <f>(F32 +(F20*F32))</f>
+        <v>144</v>
+      </c>
+      <c r="G44">
+        <f>(G32+(G20 *G32))</f>
+        <v>141</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ref="H44" si="1">(H32 +(H20*H32))</f>
+        <v>138</v>
+      </c>
+      <c r="I44">
+        <f t="shared" ref="I44" si="2">(I32+(I20 *I32))</f>
+        <v>135</v>
+      </c>
+      <c r="J44">
+        <f t="shared" ref="J44" si="3">(J32 +(J20*J32))</f>
+        <v>132</v>
+      </c>
+      <c r="K44">
+        <f t="shared" ref="K44" si="4">(K32+(K20 *K32))</f>
+        <v>129</v>
+      </c>
+      <c r="L44">
+        <f t="shared" ref="L44" si="5">(L32 +(L20*L32))</f>
+        <v>126.84</v>
+      </c>
+      <c r="M44">
+        <f t="shared" ref="M44" si="6">(M32+(M20 *M32))</f>
+        <v>124.64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <f>(E33 + (E21 * E33))</f>
+        <v>107.14993072</v>
+      </c>
+      <c r="F45">
+        <f>(F33 +(F21*F33))</f>
+        <v>98.665405593599985</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ref="G45" si="7">(G33 + (G21 * G33))</f>
+        <v>90.813283731775982</v>
+      </c>
+      <c r="H45">
+        <f t="shared" ref="H45" si="8">(H33 +(H21*H33))</f>
+        <v>83.548221033233901</v>
+      </c>
+      <c r="I45">
+        <f t="shared" ref="I45" si="9">(I33 + (I21 * I33))</f>
+        <v>76.828038037082479</v>
+      </c>
+      <c r="J45">
+        <f t="shared" ref="J45" si="10">(J33 +(J21*J33))</f>
+        <v>70.613503404749579</v>
+      </c>
+      <c r="K45">
+        <f t="shared" ref="K45" si="11">(K33 + (K21 * K33))</f>
+        <v>64.868131991363128</v>
+      </c>
+      <c r="L45">
+        <f t="shared" ref="L45" si="12">(L33 +(L21*L33))</f>
+        <v>59.557996535325962</v>
+      </c>
+      <c r="M45">
+        <f t="shared" ref="M45" si="13">(M33 + (M21 * M33))</f>
+        <v>54.651552058844345</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
+      </c>
+      <c r="C46" s="5">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0</v>
+      </c>
+      <c r="K46" s="5">
+        <v>0</v>
+      </c>
+      <c r="L46" s="5">
+        <v>0</v>
+      </c>
+      <c r="M46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <f>(E35 + (E23 * E35))</f>
+        <v>129.88919999999999</v>
+      </c>
+      <c r="F47">
+        <f>(F35 +(F23* F35))</f>
+        <v>119.60409599999998</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47" si="14">(G35 + (G23 * G35))</f>
+        <v>110.08560335999998</v>
+      </c>
+      <c r="H47">
+        <f t="shared" ref="H47" si="15">(H35 +(H23* H35))</f>
+        <v>101.27875509119998</v>
+      </c>
+      <c r="I47">
+        <f t="shared" ref="I47" si="16">(I35 + (I23 * I35))</f>
+        <v>93.132420442559976</v>
+      </c>
+      <c r="J47">
+        <f t="shared" ref="J47" si="17">(J35 +(J23* J35))</f>
+        <v>85.599042433428451</v>
+      </c>
+      <c r="K47">
+        <f t="shared" ref="K47" si="18">(K35 + (K23 * K35))</f>
+        <v>78.634393071799494</v>
+      </c>
+      <c r="L47">
+        <f t="shared" ref="L47" si="19">(L35 +(L23* L35))</f>
+        <v>69.125117630558634</v>
+      </c>
+      <c r="M47">
+        <f>(M35 + (M23 * M35))</f>
+        <v>60.731353346847939</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
+      <c r="C48" s="5">
+        <v>0</v>
+      </c>
+      <c r="D48" s="5">
+        <v>0</v>
+      </c>
+      <c r="E48" s="5">
+        <v>0</v>
+      </c>
+      <c r="F48" s="5">
+        <v>0</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0</v>
+      </c>
+      <c r="H48" s="5">
+        <v>0</v>
+      </c>
+      <c r="I48" s="5">
+        <v>0</v>
+      </c>
+      <c r="J48" s="5">
+        <v>0</v>
+      </c>
+      <c r="K48" s="5">
+        <v>0</v>
+      </c>
+      <c r="L48" s="5">
+        <v>0</v>
+      </c>
+      <c r="M48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5">
+        <v>0</v>
+      </c>
+      <c r="D49" s="5">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <f>(E36 +(E23*E36))</f>
+        <v>92.12</v>
+      </c>
+      <c r="F49">
+        <f>(F37 +(F25*F37))</f>
+        <v>199.34015999999997</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ref="G49" si="20">(G36 +(G23*G36))</f>
+        <v>78.074895999999995</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ref="H49" si="21">(H37 +(H25*H37))</f>
+        <v>168.79792515199995</v>
+      </c>
+      <c r="I49">
+        <f t="shared" ref="I49" si="22">(I36 +(I23*I36))</f>
+        <v>66.05136201599997</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ref="J49" si="23">(J37 +(J25*J37))</f>
+        <v>142.66507072238073</v>
+      </c>
+      <c r="K49">
+        <f t="shared" ref="K49" si="24">(K36 +(K23*K36))</f>
+        <v>55.769073100567013</v>
+      </c>
+      <c r="L49">
+        <f t="shared" ref="L49" si="25">(L37 +(L25*L37))</f>
+        <v>115.20852938426435</v>
+      </c>
+      <c r="M49">
+        <f t="shared" ref="M49" si="26">(M36 +(M23*M36))</f>
+        <v>46.985573782746542</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
+      <c r="C50" s="5">
+        <v>0</v>
+      </c>
+      <c r="D50" s="5">
+        <v>0</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0</v>
+      </c>
+      <c r="F50" s="5">
+        <v>0</v>
+      </c>
+      <c r="G50" s="5">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5">
+        <v>0</v>
+      </c>
+      <c r="I50" s="5">
+        <v>0</v>
+      </c>
+      <c r="J50" s="5">
+        <v>0</v>
+      </c>
+      <c r="K50" s="5">
+        <v>0</v>
+      </c>
+      <c r="L50" s="5">
+        <v>0</v>
+      </c>
+      <c r="M50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0</v>
+      </c>
+      <c r="C51" s="5">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0</v>
+      </c>
+      <c r="F51" s="5">
+        <v>0</v>
+      </c>
+      <c r="G51" s="5">
+        <v>0</v>
+      </c>
+      <c r="H51" s="5">
+        <v>0</v>
+      </c>
+      <c r="I51" s="5">
+        <v>0</v>
+      </c>
+      <c r="J51" s="5">
+        <v>0</v>
+      </c>
+      <c r="K51" s="5">
+        <v>0</v>
+      </c>
+      <c r="L51" s="5">
+        <v>0</v>
+      </c>
+      <c r="M51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <f>(E40+(E28*E40))</f>
+        <v>69.274239999999992</v>
+      </c>
+      <c r="F52">
+        <f>(F40 +(F28*F40))</f>
+        <v>63.788851199999982</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ref="G52" si="27">(G40+(G28*G40))</f>
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <f t="shared" ref="H52" si="28">(H40 +(H28*H40))</f>
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <f t="shared" ref="I52" si="29">(I40+(I28*I40))</f>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <f t="shared" ref="J52" si="30">(J40 +(J28*J40))</f>
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <f t="shared" ref="K52" si="31">(K40+(K28*K40))</f>
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <f t="shared" ref="L52" si="32">(L40 +(L28*L40))</f>
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <f t="shared" ref="M52" si="33">(M40+(M28*M40))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="5">
+        <v>0</v>
+      </c>
+      <c r="C53" s="5">
+        <v>0</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f>(E41 +(E29*E41))</f>
+        <v>49</v>
+      </c>
+      <c r="F53" s="5">
+        <f>(F41 +(F29 +F41))</f>
+        <v>99.960000000000008</v>
+      </c>
+      <c r="G53">
+        <f t="shared" ref="G53" si="34">(G41 +(G29*G41))</f>
+        <v>47</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" ref="H53" si="35">(H41 +(H29 +H41))</f>
+        <v>99.92</v>
+      </c>
+      <c r="I53">
+        <f t="shared" ref="I53" si="36">(I41 +(I29*I41))</f>
+        <v>45</v>
+      </c>
+      <c r="J53" s="5">
+        <f t="shared" ref="J53" si="37">(J41 +(J29 +J41))</f>
+        <v>99.88</v>
+      </c>
+      <c r="K53">
+        <f t="shared" ref="K53" si="38">(K41 +(K29*K41))</f>
+        <v>43</v>
+      </c>
+      <c r="L53" s="5">
+        <f t="shared" ref="L53" si="39">(L41 +(L29 +L41))</f>
+        <v>99.84</v>
+      </c>
+      <c r="M53">
+        <f t="shared" ref="M53" si="40">(M41 +(M29*M41))</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0</v>
+      </c>
+      <c r="C54" s="5">
+        <v>0</v>
+      </c>
+      <c r="D54" s="5">
+        <v>0</v>
+      </c>
+      <c r="E54" s="5">
+        <v>0</v>
+      </c>
+      <c r="F54" s="5">
+        <v>0</v>
+      </c>
+      <c r="G54" s="5">
+        <v>0</v>
+      </c>
+      <c r="H54" s="5">
+        <v>0</v>
+      </c>
+      <c r="I54" s="5">
+        <v>0</v>
+      </c>
+      <c r="J54" s="5">
+        <v>0</v>
+      </c>
+      <c r="K54" s="5">
+        <v>0</v>
+      </c>
+      <c r="L54" s="5">
+        <v>0</v>
+      </c>
+      <c r="M54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0</v>
+      </c>
+      <c r="C56" s="5">
+        <v>0</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <f>SUM(E44:E54)</f>
+        <v>594.43337071999997</v>
+      </c>
+      <c r="F56">
+        <f>SUM(F44:F54)</f>
+        <v>725.35851279359986</v>
+      </c>
+      <c r="G56">
+        <f t="shared" ref="G56:M56" si="41">SUM(G44:G54)</f>
+        <v>466.973783091776</v>
+      </c>
+      <c r="H56">
+        <f>SUM(H44:H54)</f>
+        <v>591.54490127643385</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="41"/>
+        <v>416.01182049564244</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="41"/>
+        <v>530.75761656055874</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="41"/>
+        <v>371.27159816372966</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="41"/>
+        <v>470.57164355014902</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="41"/>
+        <v>328.0084791884388</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="4">
+        <v>1272</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1388.74</v>
+      </c>
+      <c r="D57" s="4">
+        <v>1414.5955999999999</v>
+      </c>
+      <c r="E57" s="4">
+        <v>1379.919864</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1357.9246721599998</v>
+      </c>
+      <c r="G57" s="4">
+        <v>1255.9892750303998</v>
+      </c>
+      <c r="H57" s="4">
+        <v>1222.6299185285759</v>
+      </c>
+      <c r="I57" s="4">
+        <v>1191.2721234168612</v>
+      </c>
+      <c r="J57" s="4">
+        <v>1161.7957960118492</v>
+      </c>
+      <c r="K57" s="4">
+        <v>1134.0880482511386</v>
+      </c>
+      <c r="L57" s="4">
+        <v>1099.2896623394129</v>
+      </c>
+      <c r="M57" s="4">
+        <v>1067.6144898840566</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
+        <v>0</v>
+      </c>
+      <c r="C58" s="5">
+        <v>0</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2025</v>
+      </c>
+      <c r="G59" s="1">
+        <v>2026</v>
+      </c>
+      <c r="H59" s="1">
+        <v>2027</v>
+      </c>
+      <c r="I59" s="1">
+        <v>2028</v>
+      </c>
+      <c r="J59" s="1">
+        <v>2029</v>
+      </c>
+      <c r="K59" s="1">
+        <v>2030</v>
+      </c>
+      <c r="L59" s="1">
+        <v>2031</v>
+      </c>
+      <c r="M59" s="1">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0.01</v>
+      </c>
+      <c r="E60">
+        <v>0.02</v>
+      </c>
+      <c r="F60">
+        <v>0.03</v>
+      </c>
+      <c r="G60">
+        <v>0.04</v>
+      </c>
+      <c r="H60">
+        <v>0.05</v>
+      </c>
+      <c r="I60">
+        <v>0.1</v>
+      </c>
+      <c r="J60">
+        <v>0.15</v>
+      </c>
+      <c r="K60">
+        <v>0.2</v>
+      </c>
+      <c r="L60">
+        <v>0.2</v>
+      </c>
+      <c r="M60">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0.01</v>
+      </c>
+      <c r="E61">
+        <v>0.02</v>
+      </c>
+      <c r="F61">
+        <v>0.03</v>
+      </c>
+      <c r="G61">
+        <v>0.04</v>
+      </c>
+      <c r="H61">
+        <v>0.05</v>
+      </c>
+      <c r="I61">
+        <v>0.08</v>
+      </c>
+      <c r="J61">
+        <v>0.12</v>
+      </c>
+      <c r="K61">
+        <v>0.15</v>
+      </c>
+      <c r="L61">
+        <v>0.18</v>
+      </c>
+      <c r="M61">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0.01</v>
+      </c>
+      <c r="E62">
+        <v>0.02</v>
+      </c>
+      <c r="F62">
+        <v>0.03</v>
+      </c>
+      <c r="G62">
+        <v>0.04</v>
+      </c>
+      <c r="H62">
+        <v>0.05</v>
+      </c>
+      <c r="I62">
+        <v>0.06</v>
+      </c>
+      <c r="J62">
+        <v>0.08</v>
+      </c>
+      <c r="K62">
+        <v>0.1</v>
+      </c>
+      <c r="L62">
+        <v>0.12</v>
+      </c>
+      <c r="M62">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E63">
+        <v>0.01</v>
+      </c>
+      <c r="F63">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G63">
+        <v>0.02</v>
+      </c>
+      <c r="H63">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I63">
+        <v>0.03</v>
+      </c>
+      <c r="J63">
+        <v>0.04</v>
+      </c>
+      <c r="K63">
+        <v>0.05</v>
+      </c>
+      <c r="L63">
+        <v>0.06</v>
+      </c>
+      <c r="M63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1413,7 +4408,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,8 +4876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B472579F-DC66-4E5F-A641-05A694AD2961}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,8 +5299,8 @@
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
-        <v>0.48997594226142743</v>
+      <c r="B11" s="5">
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0.52495066036182003</v>
@@ -2351,8 +5346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4519566E-0386-4C17-A510-5F21C1FC657C}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>